<commit_message>
Automatische sync: 2025-06-16 23:44:18
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-16.xlsx
+++ b/logs/mail_log_2025-06-16.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1174,8 +1174,224 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw interesse. Onze openingstijden zijn maandag tot en met vrijdag van 9:00 tot 18:00 uur en op zaterdag van 10:00 tot 16:00 uur. Op zondag zijn we gesloten. Mocht u verdere vragen hebben, dan helpen we u graag verder.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:50</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:51</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:51</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant, 
+Bedankt voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 09:00 tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 17:00 uur. Op zondag zijn wij gesloten. 
+Met vriendelijke groet, 
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:54</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:54</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Bedankt voor je bericht. Onze openingstijden zijn van maandag t/m vrijdag van 9.00 uur tot 18.00 uur. Op zaterdag zijn we geopend van 10.00 uur tot 15.00 uur. Op zondag zijn we gesloten. Mocht je nog verdere vragen hebben, laat het ons gerust weten.
+Met vriendelijke groet,
+[Naam Bedrijf]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-16 23:41:57</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1195,7 +1411,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1213,7 +1429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1240,13 +1456,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1256,11 +1472,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1270,6 +1486,16 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>